<commit_message>
Data driven using Excel
</commit_message>
<xml_diff>
--- a/Data_Driven_001.xlsx
+++ b/Data_Driven_001.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">FIRST NAME</t>
   </si>
@@ -30,54 +30,18 @@
     <t xml:space="preserve">LAST NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">MARITAL STATUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOBBY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNTRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE OF BIRTH</t>
-  </si>
-  <si>
     <t xml:space="preserve">PHONE NUMBER</t>
   </si>
   <si>
-    <t xml:space="preserve">USERNAME</t>
-  </si>
-  <si>
     <t xml:space="preserve">E-mail</t>
   </si>
   <si>
-    <t xml:space="preserve">PASSWORD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONFIRM PASSWORD</t>
-  </si>
-  <si>
     <t xml:space="preserve">EMMA</t>
   </si>
   <si>
     <t xml:space="preserve">WATSON</t>
   </si>
   <si>
-    <t xml:space="preserve">SINGLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12-5-1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emmaaaarrr4545</t>
-  </si>
-  <si>
     <t xml:space="preserve">emmassdsd2354@sdasd.asd</t>
   </si>
   <si>
@@ -85,18 +49,6 @@
   </si>
   <si>
     <t xml:space="preserve">Craig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARRIED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">READING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12-5-1978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">danieladasd234a</t>
   </si>
   <si>
     <t xml:space="preserve">danielasd7231asd23@asd.asd</t>
@@ -218,26 +170,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,102 +198,39 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>1234567890</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>12345678</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>12345678</v>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>9876543210</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>12345678</v>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>12345678</v>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="emmassdsd2354@sdasd.asd"/>
-    <hyperlink ref="I3" r:id="rId2" display="danielasd7231asd23@asd.asd"/>
+    <hyperlink ref="D2" r:id="rId1" display="emmassdsd2354@sdasd.asd"/>
+    <hyperlink ref="D3" r:id="rId2" display="danielasd7231asd23@asd.asd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>